<commit_message>
Deploying to gh-pages from @ codeforIATI/codelists@56214b660bf2557f2d99cb7c193581a1aef67d30 🚀
</commit_message>
<xml_diff>
--- a/api/1/clv2/xlsx/en/SectorGroup.xlsx
+++ b/api/1/clv2/xlsx/en/SectorGroup.xlsx
@@ -31,12 +31,12 @@
     <t>codeforiati:group-name</t>
   </si>
   <si>
+    <t>codeforiati:category-name</t>
+  </si>
+  <si>
     <t>codeforiati:category-code</t>
   </si>
   <si>
-    <t>codeforiati:category-name</t>
-  </si>
-  <si>
     <t>11110</t>
   </si>
   <si>
@@ -52,12 +52,12 @@
     <t>Education</t>
   </si>
   <si>
+    <t>Education, Level Unspecified</t>
+  </si>
+  <si>
     <t>111</t>
   </si>
   <si>
-    <t>Education, Level Unspecified</t>
-  </si>
-  <si>
     <t>11120</t>
   </si>
   <si>
@@ -82,12 +82,12 @@
     <t>Primary education</t>
   </si>
   <si>
+    <t>Basic Education</t>
+  </si>
+  <si>
     <t>112</t>
   </si>
   <si>
-    <t>Basic Education</t>
-  </si>
-  <si>
     <t>11230</t>
   </si>
   <si>
@@ -130,12 +130,12 @@
     <t>Upper Secondary Education (modified and includes data from 11322)</t>
   </si>
   <si>
+    <t>Secondary Education</t>
+  </si>
+  <si>
     <t>113</t>
   </si>
   <si>
-    <t>Secondary Education</t>
-  </si>
-  <si>
     <t>11330</t>
   </si>
   <si>
@@ -148,12 +148,12 @@
     <t>Higher education</t>
   </si>
   <si>
+    <t>Post-Secondary Education</t>
+  </si>
+  <si>
     <t>114</t>
   </si>
   <si>
-    <t>Post-Secondary Education</t>
-  </si>
-  <si>
     <t>11430</t>
   </si>
   <si>
@@ -172,12 +172,12 @@
     <t>Health</t>
   </si>
   <si>
+    <t>Health, General</t>
+  </si>
+  <si>
     <t>121</t>
   </si>
   <si>
-    <t>Health, General</t>
-  </si>
-  <si>
     <t>12181</t>
   </si>
   <si>
@@ -202,12 +202,12 @@
     <t>Basic health care</t>
   </si>
   <si>
+    <t>Basic Health</t>
+  </si>
+  <si>
     <t>122</t>
   </si>
   <si>
-    <t>Basic Health</t>
-  </si>
-  <si>
     <t>12230</t>
   </si>
   <si>
@@ -262,12 +262,12 @@
     <t>NCDs control, general</t>
   </si>
   <si>
+    <t>Non-communicable diseases (NCDs)</t>
+  </si>
+  <si>
     <t>123</t>
   </si>
   <si>
-    <t>Non-communicable diseases (NCDs)</t>
-  </si>
-  <si>
     <t>12320</t>
   </si>
   <si>
@@ -418,12 +418,12 @@
     <t>Government &amp; Civil Society</t>
   </si>
   <si>
+    <t>Government &amp; Civil Society-general</t>
+  </si>
+  <si>
     <t>151</t>
   </si>
   <si>
-    <t>Government &amp; Civil Society-general</t>
-  </si>
-  <si>
     <t>15111</t>
   </si>
   <si>
@@ -520,12 +520,12 @@
     <t>Security system management and reform</t>
   </si>
   <si>
+    <t>Conflict, Peace &amp; Security</t>
+  </si>
+  <si>
     <t>152</t>
   </si>
   <si>
-    <t>Conflict, Peace &amp; Security</t>
-  </si>
-  <si>
     <t>15220</t>
   </si>
   <si>
@@ -718,12 +718,12 @@
     <t>Energy</t>
   </si>
   <si>
+    <t>Energy Policy</t>
+  </si>
+  <si>
     <t>231</t>
   </si>
   <si>
-    <t>Energy Policy</t>
-  </si>
-  <si>
     <t>23181</t>
   </si>
   <si>
@@ -748,12 +748,12 @@
     <t>Energy generation, renewable sources - multiple technologies</t>
   </si>
   <si>
+    <t>Energy generation, renewable sources</t>
+  </si>
+  <si>
     <t>232</t>
   </si>
   <si>
-    <t>Energy generation, renewable sources</t>
-  </si>
-  <si>
     <t>23220</t>
   </si>
   <si>
@@ -808,12 +808,12 @@
     <t>Energy generation, non-renewable sources, unspecified</t>
   </si>
   <si>
+    <t>Energy generation, non-renewable sources</t>
+  </si>
+  <si>
     <t>233</t>
   </si>
   <si>
-    <t>Energy generation, non-renewable sources</t>
-  </si>
-  <si>
     <t>23320</t>
   </si>
   <si>
@@ -850,36 +850,36 @@
     <t>Hybrid energy electric power plants</t>
   </si>
   <si>
+    <t>Hybrid energy plants</t>
+  </si>
+  <si>
     <t>234</t>
   </si>
   <si>
-    <t>Hybrid energy plants</t>
-  </si>
-  <si>
     <t>23510</t>
   </si>
   <si>
     <t>Nuclear energy electric power plants and nuclear safety</t>
   </si>
   <si>
+    <t>Nuclear energy plants</t>
+  </si>
+  <si>
     <t>235</t>
   </si>
   <si>
-    <t>Nuclear energy plants</t>
-  </si>
-  <si>
     <t>23610</t>
   </si>
   <si>
     <t>Heat plants</t>
   </si>
   <si>
+    <t>Energy distribution</t>
+  </si>
+  <si>
     <t>236</t>
   </si>
   <si>
-    <t>Energy distribution</t>
-  </si>
-  <si>
     <t>23620</t>
   </si>
   <si>
@@ -1000,12 +1000,12 @@
     <t>Agriculture, Forestry, Fishing</t>
   </si>
   <si>
+    <t>Agriculture</t>
+  </si>
+  <si>
     <t>311</t>
   </si>
   <si>
-    <t>Agriculture</t>
-  </si>
-  <si>
     <t>31120</t>
   </si>
   <si>
@@ -1114,12 +1114,12 @@
     <t>Forestry policy and administrative management</t>
   </si>
   <si>
+    <t>Forestry</t>
+  </si>
+  <si>
     <t>312</t>
   </si>
   <si>
-    <t>Forestry</t>
-  </si>
-  <si>
     <t>31220</t>
   </si>
   <si>
@@ -1156,12 +1156,12 @@
     <t>Fishing policy and administrative management</t>
   </si>
   <si>
+    <t>Fishing</t>
+  </si>
+  <si>
     <t>313</t>
   </si>
   <si>
-    <t>Fishing</t>
-  </si>
-  <si>
     <t>31320</t>
   </si>
   <si>
@@ -1198,12 +1198,12 @@
     <t>Industry, Mining, Construction</t>
   </si>
   <si>
+    <t>Industry</t>
+  </si>
+  <si>
     <t>321</t>
   </si>
   <si>
-    <t>Industry</t>
-  </si>
-  <si>
     <t>32120</t>
   </si>
   <si>
@@ -1318,12 +1318,12 @@
     <t>Mineral/mining policy and administrative management</t>
   </si>
   <si>
+    <t>Mineral Resources &amp; Mining</t>
+  </si>
+  <si>
     <t>322</t>
   </si>
   <si>
-    <t>Mineral Resources &amp; Mining</t>
-  </si>
-  <si>
     <t>32220</t>
   </si>
   <si>
@@ -1384,10 +1384,10 @@
     <t>Construction policy and administrative management</t>
   </si>
   <si>
+    <t>Construction</t>
+  </si>
+  <si>
     <t>323</t>
-  </si>
-  <si>
-    <t>Construction</t>
   </si>
   <si>
     <t>33110</t>
@@ -2889,10 +2889,10 @@
         <v>97</v>
       </c>
       <c r="F36" t="s">
+        <v>97</v>
+      </c>
+      <c r="G36" t="s">
         <v>96</v>
-      </c>
-      <c r="G36" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -2912,10 +2912,10 @@
         <v>97</v>
       </c>
       <c r="F37" t="s">
+        <v>97</v>
+      </c>
+      <c r="G37" t="s">
         <v>96</v>
-      </c>
-      <c r="G37" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -2935,10 +2935,10 @@
         <v>97</v>
       </c>
       <c r="F38" t="s">
+        <v>97</v>
+      </c>
+      <c r="G38" t="s">
         <v>96</v>
-      </c>
-      <c r="G38" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -2958,10 +2958,10 @@
         <v>97</v>
       </c>
       <c r="F39" t="s">
+        <v>97</v>
+      </c>
+      <c r="G39" t="s">
         <v>96</v>
-      </c>
-      <c r="G39" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -2981,10 +2981,10 @@
         <v>97</v>
       </c>
       <c r="F40" t="s">
+        <v>97</v>
+      </c>
+      <c r="G40" t="s">
         <v>96</v>
-      </c>
-      <c r="G40" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -3004,10 +3004,10 @@
         <v>109</v>
       </c>
       <c r="F41" t="s">
+        <v>109</v>
+      </c>
+      <c r="G41" t="s">
         <v>108</v>
-      </c>
-      <c r="G41" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -3027,10 +3027,10 @@
         <v>109</v>
       </c>
       <c r="F42" t="s">
+        <v>109</v>
+      </c>
+      <c r="G42" t="s">
         <v>108</v>
-      </c>
-      <c r="G42" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -3050,10 +3050,10 @@
         <v>109</v>
       </c>
       <c r="F43" t="s">
+        <v>109</v>
+      </c>
+      <c r="G43" t="s">
         <v>108</v>
-      </c>
-      <c r="G43" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -3073,10 +3073,10 @@
         <v>109</v>
       </c>
       <c r="F44" t="s">
+        <v>109</v>
+      </c>
+      <c r="G44" t="s">
         <v>108</v>
-      </c>
-      <c r="G44" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -3096,10 +3096,10 @@
         <v>109</v>
       </c>
       <c r="F45" t="s">
+        <v>109</v>
+      </c>
+      <c r="G45" t="s">
         <v>108</v>
-      </c>
-      <c r="G45" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -3119,10 +3119,10 @@
         <v>109</v>
       </c>
       <c r="F46" t="s">
+        <v>109</v>
+      </c>
+      <c r="G46" t="s">
         <v>108</v>
-      </c>
-      <c r="G46" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -3142,10 +3142,10 @@
         <v>109</v>
       </c>
       <c r="F47" t="s">
+        <v>109</v>
+      </c>
+      <c r="G47" t="s">
         <v>108</v>
-      </c>
-      <c r="G47" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -3165,10 +3165,10 @@
         <v>109</v>
       </c>
       <c r="F48" t="s">
+        <v>109</v>
+      </c>
+      <c r="G48" t="s">
         <v>108</v>
-      </c>
-      <c r="G48" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -3188,10 +3188,10 @@
         <v>109</v>
       </c>
       <c r="F49" t="s">
+        <v>109</v>
+      </c>
+      <c r="G49" t="s">
         <v>108</v>
-      </c>
-      <c r="G49" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -3211,10 +3211,10 @@
         <v>109</v>
       </c>
       <c r="F50" t="s">
+        <v>109</v>
+      </c>
+      <c r="G50" t="s">
         <v>108</v>
-      </c>
-      <c r="G50" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -3234,10 +3234,10 @@
         <v>109</v>
       </c>
       <c r="F51" t="s">
+        <v>109</v>
+      </c>
+      <c r="G51" t="s">
         <v>108</v>
-      </c>
-      <c r="G51" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -3763,10 +3763,10 @@
         <v>183</v>
       </c>
       <c r="F74" t="s">
+        <v>183</v>
+      </c>
+      <c r="G74" t="s">
         <v>182</v>
-      </c>
-      <c r="G74" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -3786,10 +3786,10 @@
         <v>183</v>
       </c>
       <c r="F75" t="s">
+        <v>183</v>
+      </c>
+      <c r="G75" t="s">
         <v>182</v>
-      </c>
-      <c r="G75" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -3809,10 +3809,10 @@
         <v>183</v>
       </c>
       <c r="F76" t="s">
+        <v>183</v>
+      </c>
+      <c r="G76" t="s">
         <v>182</v>
-      </c>
-      <c r="G76" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -3832,10 +3832,10 @@
         <v>183</v>
       </c>
       <c r="F77" t="s">
+        <v>183</v>
+      </c>
+      <c r="G77" t="s">
         <v>182</v>
-      </c>
-      <c r="G77" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -3855,10 +3855,10 @@
         <v>183</v>
       </c>
       <c r="F78" t="s">
+        <v>183</v>
+      </c>
+      <c r="G78" t="s">
         <v>182</v>
-      </c>
-      <c r="G78" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -3878,10 +3878,10 @@
         <v>183</v>
       </c>
       <c r="F79" t="s">
+        <v>183</v>
+      </c>
+      <c r="G79" t="s">
         <v>182</v>
-      </c>
-      <c r="G79" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -3901,10 +3901,10 @@
         <v>183</v>
       </c>
       <c r="F80" t="s">
+        <v>183</v>
+      </c>
+      <c r="G80" t="s">
         <v>182</v>
-      </c>
-      <c r="G80" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -3924,10 +3924,10 @@
         <v>183</v>
       </c>
       <c r="F81" t="s">
+        <v>183</v>
+      </c>
+      <c r="G81" t="s">
         <v>182</v>
-      </c>
-      <c r="G81" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -3947,10 +3947,10 @@
         <v>183</v>
       </c>
       <c r="F82" t="s">
+        <v>183</v>
+      </c>
+      <c r="G82" t="s">
         <v>182</v>
-      </c>
-      <c r="G82" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -3970,10 +3970,10 @@
         <v>183</v>
       </c>
       <c r="F83" t="s">
+        <v>183</v>
+      </c>
+      <c r="G83" t="s">
         <v>182</v>
-      </c>
-      <c r="G83" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -3993,10 +3993,10 @@
         <v>183</v>
       </c>
       <c r="F84" t="s">
+        <v>183</v>
+      </c>
+      <c r="G84" t="s">
         <v>182</v>
-      </c>
-      <c r="G84" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -4016,10 +4016,10 @@
         <v>207</v>
       </c>
       <c r="F85" t="s">
+        <v>207</v>
+      </c>
+      <c r="G85" t="s">
         <v>206</v>
-      </c>
-      <c r="G85" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -4039,10 +4039,10 @@
         <v>207</v>
       </c>
       <c r="F86" t="s">
+        <v>207</v>
+      </c>
+      <c r="G86" t="s">
         <v>206</v>
-      </c>
-      <c r="G86" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -4062,10 +4062,10 @@
         <v>207</v>
       </c>
       <c r="F87" t="s">
+        <v>207</v>
+      </c>
+      <c r="G87" t="s">
         <v>206</v>
-      </c>
-      <c r="G87" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -4085,10 +4085,10 @@
         <v>207</v>
       </c>
       <c r="F88" t="s">
+        <v>207</v>
+      </c>
+      <c r="G88" t="s">
         <v>206</v>
-      </c>
-      <c r="G88" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -4108,10 +4108,10 @@
         <v>207</v>
       </c>
       <c r="F89" t="s">
+        <v>207</v>
+      </c>
+      <c r="G89" t="s">
         <v>206</v>
-      </c>
-      <c r="G89" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -4131,10 +4131,10 @@
         <v>207</v>
       </c>
       <c r="F90" t="s">
+        <v>207</v>
+      </c>
+      <c r="G90" t="s">
         <v>206</v>
-      </c>
-      <c r="G90" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -4154,10 +4154,10 @@
         <v>207</v>
       </c>
       <c r="F91" t="s">
+        <v>207</v>
+      </c>
+      <c r="G91" t="s">
         <v>206</v>
-      </c>
-      <c r="G91" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -4177,10 +4177,10 @@
         <v>223</v>
       </c>
       <c r="F92" t="s">
+        <v>223</v>
+      </c>
+      <c r="G92" t="s">
         <v>222</v>
-      </c>
-      <c r="G92" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -4200,10 +4200,10 @@
         <v>223</v>
       </c>
       <c r="F93" t="s">
+        <v>223</v>
+      </c>
+      <c r="G93" t="s">
         <v>222</v>
-      </c>
-      <c r="G93" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -4223,10 +4223,10 @@
         <v>223</v>
       </c>
       <c r="F94" t="s">
+        <v>223</v>
+      </c>
+      <c r="G94" t="s">
         <v>222</v>
-      </c>
-      <c r="G94" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -4246,10 +4246,10 @@
         <v>223</v>
       </c>
       <c r="F95" t="s">
+        <v>223</v>
+      </c>
+      <c r="G95" t="s">
         <v>222</v>
-      </c>
-      <c r="G95" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -4913,10 +4913,10 @@
         <v>303</v>
       </c>
       <c r="F124" t="s">
+        <v>303</v>
+      </c>
+      <c r="G124" t="s">
         <v>302</v>
-      </c>
-      <c r="G124" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="125" spans="1:7">
@@ -4936,10 +4936,10 @@
         <v>303</v>
       </c>
       <c r="F125" t="s">
+        <v>303</v>
+      </c>
+      <c r="G125" t="s">
         <v>302</v>
-      </c>
-      <c r="G125" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="126" spans="1:7">
@@ -4959,10 +4959,10 @@
         <v>303</v>
       </c>
       <c r="F126" t="s">
+        <v>303</v>
+      </c>
+      <c r="G126" t="s">
         <v>302</v>
-      </c>
-      <c r="G126" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="127" spans="1:7">
@@ -4982,10 +4982,10 @@
         <v>303</v>
       </c>
       <c r="F127" t="s">
+        <v>303</v>
+      </c>
+      <c r="G127" t="s">
         <v>302</v>
-      </c>
-      <c r="G127" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="128" spans="1:7">
@@ -5005,10 +5005,10 @@
         <v>303</v>
       </c>
       <c r="F128" t="s">
+        <v>303</v>
+      </c>
+      <c r="G128" t="s">
         <v>302</v>
-      </c>
-      <c r="G128" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="129" spans="1:7">
@@ -5028,10 +5028,10 @@
         <v>303</v>
       </c>
       <c r="F129" t="s">
+        <v>303</v>
+      </c>
+      <c r="G129" t="s">
         <v>302</v>
-      </c>
-      <c r="G129" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="130" spans="1:7">
@@ -5051,10 +5051,10 @@
         <v>317</v>
       </c>
       <c r="F130" t="s">
+        <v>317</v>
+      </c>
+      <c r="G130" t="s">
         <v>316</v>
-      </c>
-      <c r="G130" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="131" spans="1:7">
@@ -5074,10 +5074,10 @@
         <v>317</v>
       </c>
       <c r="F131" t="s">
+        <v>317</v>
+      </c>
+      <c r="G131" t="s">
         <v>316</v>
-      </c>
-      <c r="G131" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="132" spans="1:7">
@@ -5097,10 +5097,10 @@
         <v>317</v>
       </c>
       <c r="F132" t="s">
+        <v>317</v>
+      </c>
+      <c r="G132" t="s">
         <v>316</v>
-      </c>
-      <c r="G132" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="133" spans="1:7">
@@ -5120,10 +5120,10 @@
         <v>317</v>
       </c>
       <c r="F133" t="s">
+        <v>317</v>
+      </c>
+      <c r="G133" t="s">
         <v>316</v>
-      </c>
-      <c r="G133" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="134" spans="1:7">
@@ -6500,10 +6500,10 @@
         <v>461</v>
       </c>
       <c r="F193" t="s">
+        <v>461</v>
+      </c>
+      <c r="G193" t="s">
         <v>460</v>
-      </c>
-      <c r="G193" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="194" spans="1:7">
@@ -6523,10 +6523,10 @@
         <v>461</v>
       </c>
       <c r="F194" t="s">
+        <v>461</v>
+      </c>
+      <c r="G194" t="s">
         <v>460</v>
-      </c>
-      <c r="G194" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="195" spans="1:7">
@@ -6546,10 +6546,10 @@
         <v>461</v>
       </c>
       <c r="F195" t="s">
+        <v>461</v>
+      </c>
+      <c r="G195" t="s">
         <v>460</v>
-      </c>
-      <c r="G195" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="196" spans="1:7">
@@ -6569,10 +6569,10 @@
         <v>461</v>
       </c>
       <c r="F196" t="s">
+        <v>461</v>
+      </c>
+      <c r="G196" t="s">
         <v>460</v>
-      </c>
-      <c r="G196" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="197" spans="1:7">
@@ -6592,10 +6592,10 @@
         <v>461</v>
       </c>
       <c r="F197" t="s">
+        <v>461</v>
+      </c>
+      <c r="G197" t="s">
         <v>460</v>
-      </c>
-      <c r="G197" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="198" spans="1:7">
@@ -6615,10 +6615,10 @@
         <v>461</v>
       </c>
       <c r="F198" t="s">
+        <v>461</v>
+      </c>
+      <c r="G198" t="s">
         <v>460</v>
-      </c>
-      <c r="G198" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="199" spans="1:7">
@@ -6638,10 +6638,10 @@
         <v>475</v>
       </c>
       <c r="F199" t="s">
+        <v>475</v>
+      </c>
+      <c r="G199" t="s">
         <v>474</v>
-      </c>
-      <c r="G199" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="200" spans="1:7">
@@ -6661,10 +6661,10 @@
         <v>479</v>
       </c>
       <c r="F200" t="s">
+        <v>479</v>
+      </c>
+      <c r="G200" t="s">
         <v>478</v>
-      </c>
-      <c r="G200" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="201" spans="1:7">
@@ -6684,10 +6684,10 @@
         <v>479</v>
       </c>
       <c r="F201" t="s">
+        <v>479</v>
+      </c>
+      <c r="G201" t="s">
         <v>478</v>
-      </c>
-      <c r="G201" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="202" spans="1:7">
@@ -6707,10 +6707,10 @@
         <v>479</v>
       </c>
       <c r="F202" t="s">
+        <v>479</v>
+      </c>
+      <c r="G202" t="s">
         <v>478</v>
-      </c>
-      <c r="G202" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="203" spans="1:7">
@@ -6730,10 +6730,10 @@
         <v>479</v>
       </c>
       <c r="F203" t="s">
+        <v>479</v>
+      </c>
+      <c r="G203" t="s">
         <v>478</v>
-      </c>
-      <c r="G203" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="204" spans="1:7">
@@ -6753,10 +6753,10 @@
         <v>479</v>
       </c>
       <c r="F204" t="s">
+        <v>479</v>
+      </c>
+      <c r="G204" t="s">
         <v>478</v>
-      </c>
-      <c r="G204" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="205" spans="1:7">
@@ -6776,10 +6776,10 @@
         <v>479</v>
       </c>
       <c r="F205" t="s">
+        <v>479</v>
+      </c>
+      <c r="G205" t="s">
         <v>478</v>
-      </c>
-      <c r="G205" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="206" spans="1:7">
@@ -6799,10 +6799,10 @@
         <v>493</v>
       </c>
       <c r="F206" t="s">
+        <v>493</v>
+      </c>
+      <c r="G206" t="s">
         <v>492</v>
-      </c>
-      <c r="G206" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="207" spans="1:7">
@@ -6822,10 +6822,10 @@
         <v>493</v>
       </c>
       <c r="F207" t="s">
+        <v>493</v>
+      </c>
+      <c r="G207" t="s">
         <v>492</v>
-      </c>
-      <c r="G207" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="208" spans="1:7">
@@ -6845,10 +6845,10 @@
         <v>493</v>
       </c>
       <c r="F208" t="s">
+        <v>493</v>
+      </c>
+      <c r="G208" t="s">
         <v>492</v>
-      </c>
-      <c r="G208" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="209" spans="1:7">
@@ -6868,10 +6868,10 @@
         <v>493</v>
       </c>
       <c r="F209" t="s">
+        <v>493</v>
+      </c>
+      <c r="G209" t="s">
         <v>492</v>
-      </c>
-      <c r="G209" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="210" spans="1:7">
@@ -6891,10 +6891,10 @@
         <v>493</v>
       </c>
       <c r="F210" t="s">
+        <v>493</v>
+      </c>
+      <c r="G210" t="s">
         <v>492</v>
-      </c>
-      <c r="G210" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="211" spans="1:7">
@@ -6914,10 +6914,10 @@
         <v>493</v>
       </c>
       <c r="F211" t="s">
+        <v>493</v>
+      </c>
+      <c r="G211" t="s">
         <v>492</v>
-      </c>
-      <c r="G211" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="212" spans="1:7">
@@ -6937,10 +6937,10 @@
         <v>493</v>
       </c>
       <c r="F212" t="s">
+        <v>493</v>
+      </c>
+      <c r="G212" t="s">
         <v>492</v>
-      </c>
-      <c r="G212" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="213" spans="1:7">
@@ -6960,10 +6960,10 @@
         <v>493</v>
       </c>
       <c r="F213" t="s">
+        <v>493</v>
+      </c>
+      <c r="G213" t="s">
         <v>492</v>
-      </c>
-      <c r="G213" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="214" spans="1:7">
@@ -6983,10 +6983,10 @@
         <v>493</v>
       </c>
       <c r="F214" t="s">
+        <v>493</v>
+      </c>
+      <c r="G214" t="s">
         <v>492</v>
-      </c>
-      <c r="G214" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="215" spans="1:7">
@@ -7006,10 +7006,10 @@
         <v>493</v>
       </c>
       <c r="F215" t="s">
+        <v>493</v>
+      </c>
+      <c r="G215" t="s">
         <v>492</v>
-      </c>
-      <c r="G215" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="216" spans="1:7">
@@ -7029,10 +7029,10 @@
         <v>515</v>
       </c>
       <c r="F216" t="s">
+        <v>515</v>
+      </c>
+      <c r="G216" t="s">
         <v>514</v>
-      </c>
-      <c r="G216" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="217" spans="1:7">
@@ -7052,10 +7052,10 @@
         <v>519</v>
       </c>
       <c r="F217" t="s">
+        <v>519</v>
+      </c>
+      <c r="G217" t="s">
         <v>518</v>
-      </c>
-      <c r="G217" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="218" spans="1:7">
@@ -7075,10 +7075,10 @@
         <v>523</v>
       </c>
       <c r="F218" t="s">
+        <v>523</v>
+      </c>
+      <c r="G218" t="s">
         <v>522</v>
-      </c>
-      <c r="G218" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="219" spans="1:7">
@@ -7098,10 +7098,10 @@
         <v>523</v>
       </c>
       <c r="F219" t="s">
+        <v>523</v>
+      </c>
+      <c r="G219" t="s">
         <v>522</v>
-      </c>
-      <c r="G219" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="220" spans="1:7">
@@ -7121,10 +7121,10 @@
         <v>529</v>
       </c>
       <c r="F220" t="s">
+        <v>529</v>
+      </c>
+      <c r="G220" t="s">
         <v>528</v>
-      </c>
-      <c r="G220" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="221" spans="1:7">
@@ -7144,10 +7144,10 @@
         <v>529</v>
       </c>
       <c r="F221" t="s">
+        <v>529</v>
+      </c>
+      <c r="G221" t="s">
         <v>528</v>
-      </c>
-      <c r="G221" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="222" spans="1:7">
@@ -7167,10 +7167,10 @@
         <v>529</v>
       </c>
       <c r="F222" t="s">
+        <v>529</v>
+      </c>
+      <c r="G222" t="s">
         <v>528</v>
-      </c>
-      <c r="G222" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="223" spans="1:7">
@@ -7190,10 +7190,10 @@
         <v>529</v>
       </c>
       <c r="F223" t="s">
+        <v>529</v>
+      </c>
+      <c r="G223" t="s">
         <v>528</v>
-      </c>
-      <c r="G223" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="224" spans="1:7">
@@ -7213,10 +7213,10 @@
         <v>529</v>
       </c>
       <c r="F224" t="s">
+        <v>529</v>
+      </c>
+      <c r="G224" t="s">
         <v>528</v>
-      </c>
-      <c r="G224" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="225" spans="1:7">
@@ -7236,10 +7236,10 @@
         <v>529</v>
       </c>
       <c r="F225" t="s">
+        <v>529</v>
+      </c>
+      <c r="G225" t="s">
         <v>528</v>
-      </c>
-      <c r="G225" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="226" spans="1:7">
@@ -7259,10 +7259,10 @@
         <v>529</v>
       </c>
       <c r="F226" t="s">
+        <v>529</v>
+      </c>
+      <c r="G226" t="s">
         <v>528</v>
-      </c>
-      <c r="G226" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="227" spans="1:7">
@@ -7282,10 +7282,10 @@
         <v>545</v>
       </c>
       <c r="F227" t="s">
+        <v>545</v>
+      </c>
+      <c r="G227" t="s">
         <v>544</v>
-      </c>
-      <c r="G227" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="228" spans="1:7">
@@ -7305,10 +7305,10 @@
         <v>545</v>
       </c>
       <c r="F228" t="s">
+        <v>545</v>
+      </c>
+      <c r="G228" t="s">
         <v>544</v>
-      </c>
-      <c r="G228" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="229" spans="1:7">
@@ -7328,10 +7328,10 @@
         <v>545</v>
       </c>
       <c r="F229" t="s">
+        <v>545</v>
+      </c>
+      <c r="G229" t="s">
         <v>544</v>
-      </c>
-      <c r="G229" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="230" spans="1:7">
@@ -7351,10 +7351,10 @@
         <v>553</v>
       </c>
       <c r="F230" t="s">
+        <v>553</v>
+      </c>
+      <c r="G230" t="s">
         <v>552</v>
-      </c>
-      <c r="G230" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="231" spans="1:7">
@@ -7374,10 +7374,10 @@
         <v>557</v>
       </c>
       <c r="F231" t="s">
+        <v>557</v>
+      </c>
+      <c r="G231" t="s">
         <v>556</v>
-      </c>
-      <c r="G231" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="232" spans="1:7">
@@ -7397,10 +7397,10 @@
         <v>561</v>
       </c>
       <c r="F232" t="s">
+        <v>561</v>
+      </c>
+      <c r="G232" t="s">
         <v>560</v>
-      </c>
-      <c r="G232" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="233" spans="1:7">
@@ -7420,10 +7420,10 @@
         <v>565</v>
       </c>
       <c r="F233" t="s">
+        <v>565</v>
+      </c>
+      <c r="G233" t="s">
         <v>564</v>
-      </c>
-      <c r="G233" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="234" spans="1:7">
@@ -7443,10 +7443,10 @@
         <v>569</v>
       </c>
       <c r="F234" t="s">
+        <v>569</v>
+      </c>
+      <c r="G234" t="s">
         <v>568</v>
-      </c>
-      <c r="G234" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="235" spans="1:7">
@@ -7466,10 +7466,10 @@
         <v>569</v>
       </c>
       <c r="F235" t="s">
+        <v>569</v>
+      </c>
+      <c r="G235" t="s">
         <v>568</v>
-      </c>
-      <c r="G235" t="s">
-        <v>569</v>
       </c>
     </row>
   </sheetData>

</xml_diff>